<commit_message>
Change Global_Parameters to include MipGap
</commit_message>
<xml_diff>
--- a/data/Szenario_Link_different/Global_Parameters.xlsx
+++ b/data/Szenario_Link_different/Global_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Server\Desktop\Michael\LEGO-Pyomo\data\Szenario_Default\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\git\LEGO-Pyomo\data\Szenario_Default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB3BFF-0D70-4CB0-9EBD-5DBD3F86E021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB5B84-779C-473B-9655-200493984165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Parameters" sheetId="121" r:id="rId1"/>
@@ -59,15 +59,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>[h]</t>
   </si>
@@ -187,6 +184,21 @@
   </si>
   <si>
     <t>Scaling factor for power values in input data (relative to 1MW)</t>
+  </si>
+  <si>
+    <t>Mip Gap</t>
+  </si>
+  <si>
+    <t>The MIP solver will terminate (with an optimal result) when the gap between the lower and upper objective bound is less than pMIPGap</t>
+  </si>
+  <si>
+    <t>pMIPGap</t>
+  </si>
+  <si>
+    <t>[%]</t>
+  </si>
+  <si>
+    <t>Relative MIP gap</t>
   </si>
   <si>
     <t>No</t>
@@ -408,16 +420,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -805,13 +831,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H19"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
@@ -824,12 +850,12 @@
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
@@ -849,7 +875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
@@ -861,12 +887,12 @@
       <c r="G4" s="11"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>24</v>
@@ -881,12 +907,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -897,12 +923,12 @@
       <c r="F7" s="11"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>9</v>
@@ -917,81 +943,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="5" t="s">
+      <c r="C13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="13">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G14" s="11"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15" s="9">
-        <v>9.9999999999999995E-7</v>
+        <v>1E-3</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>33</v>
@@ -1000,92 +1028,136 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="7" t="s">
+    <row r="16" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="13">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="5" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="3" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C22" s="9">
         <v>168</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H22" s="13">
         <v>168</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+  <conditionalFormatting sqref="C18">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8:C9" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 C12 C15" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}"/>
-    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C5 C15 C18 C11" xr:uid="{13E44DF0-E318-4006-9E46-A03D51C3BE3C}"/>
+    <dataValidation type="whole" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{B1F27E54-4BFD-2D4B-9633-37AF83A83F57}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1095,6 +1167,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1240,22 +1327,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1271,28 +1367,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>